<commit_message>
Added Sunbreak data and restructured the project so that seasons and tournaments make the same plots.  Added some statistics/plots around O/D percentage.
</commit_message>
<xml_diff>
--- a/PointData/2022_GandyGoose_Points.xlsx
+++ b/PointData/2022_GandyGoose_Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fiedl\Documents\PointAnalysis\PointData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9639C223-667E-49DE-B182-1C703EFA815C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67961DB-8B92-483F-8245-50703D999D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{880E8181-9B5F-AA4E-BF42-ACE5DA835884}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{880E8181-9B5F-AA4E-BF42-ACE5DA835884}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1 Game 1" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>Jeremy Vargas</t>
   </si>
   <si>
-    <t xml:space="preserve">Josh Zylstra </t>
-  </si>
-  <si>
     <t>Kevin Fiedler</t>
   </si>
   <si>
@@ -133,10 +130,13 @@
     <t>Sam Diedesch</t>
   </si>
   <si>
-    <t xml:space="preserve">Trevor Kilgannon </t>
+    <t>Zac Carter</t>
   </si>
   <si>
-    <t>Zac Carter</t>
+    <t>Josh Zylstra</t>
+  </si>
+  <si>
+    <t>Trevor Kilgannon</t>
   </si>
 </sst>
 </file>
@@ -491,15 +491,15 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -611,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -667,7 +667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -723,22 +723,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -761,7 +761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -787,7 +787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -819,7 +819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -848,7 +848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -868,7 +868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -888,7 +888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -908,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -931,7 +931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -960,7 +960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -968,7 +968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -991,7 +991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1049,12 +1049,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1077,115 +1077,115 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>8</v>
-      </c>
-      <c r="O23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="P25" t="s">
+        <v>8</v>
+      </c>
+      <c r="R25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" t="s">
-        <v>8</v>
-      </c>
-      <c r="P25" t="s">
-        <v>8</v>
-      </c>
-      <c r="R25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" t="s">
+        <v>8</v>
+      </c>
+      <c r="P26" t="s">
+        <v>8</v>
+      </c>
+      <c r="R26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+      <c r="P27" t="s">
+        <v>8</v>
+      </c>
+      <c r="R27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>29</v>
-      </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" t="s">
-        <v>8</v>
-      </c>
-      <c r="P26" t="s">
-        <v>8</v>
-      </c>
-      <c r="R26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" t="s">
-        <v>8</v>
-      </c>
-      <c r="M27" t="s">
-        <v>8</v>
-      </c>
-      <c r="P27" t="s">
-        <v>8</v>
-      </c>
-      <c r="R27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1209,16 +1209,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FA7185-A88C-1948-AEF7-614A2526D4FC}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D36" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1454,17 +1454,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1829,109 +1829,109 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>8</v>
-      </c>
-      <c r="R24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" t="s">
+        <v>8</v>
+      </c>
+      <c r="P25" t="s">
+        <v>8</v>
+      </c>
+      <c r="S25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" t="s">
-        <v>8</v>
-      </c>
-      <c r="O25" t="s">
-        <v>8</v>
-      </c>
-      <c r="P25" t="s">
-        <v>8</v>
-      </c>
-      <c r="S25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" t="s">
+        <v>8</v>
+      </c>
+      <c r="P26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" t="s">
-        <v>8</v>
-      </c>
-      <c r="L26" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" t="s">
-        <v>8</v>
-      </c>
-      <c r="P26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1961,16 +1961,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948B1016-AF59-4E43-B709-27199732E928}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2118,45 +2118,45 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
       <c r="J6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2395,76 +2395,76 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>29</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
-      <c r="J26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -2486,15 +2486,15 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2718,33 +2718,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="N5" t="s">
         <v>21</v>
       </c>
       <c r="P5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2755,22 +2755,22 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
         <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3114,109 +3114,109 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>8</v>
+      </c>
+      <c r="P23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" t="s">
-        <v>8</v>
-      </c>
-      <c r="P23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" t="s">
-        <v>8</v>
-      </c>
-      <c r="P24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" t="s">
+        <v>8</v>
+      </c>
+      <c r="R25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" t="s">
-        <v>8</v>
-      </c>
-      <c r="N25" t="s">
-        <v>8</v>
-      </c>
-      <c r="O25" t="s">
-        <v>8</v>
-      </c>
-      <c r="R25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" t="s">
+        <v>8</v>
+      </c>
+      <c r="L27" t="s">
+        <v>8</v>
+      </c>
+      <c r="P27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" t="s">
-        <v>8</v>
-      </c>
-      <c r="L27" t="s">
-        <v>8</v>
-      </c>
-      <c r="P27" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -3246,16 +3246,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B962C4-F174-9F47-9298-A684442E8BF5}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="J4" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3562,45 +3562,45 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K5" t="s">
         <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U5" t="s">
         <v>11</v>
       </c>
       <c r="W5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
         <v>23</v>
@@ -3615,19 +3615,19 @@
         <v>14</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q6" t="s">
         <v>19</v>
       </c>
       <c r="U6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="W6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3828,12 +3828,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3960,12 +3960,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -4049,145 +4049,145 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" t="s">
+        <v>8</v>
+      </c>
+      <c r="U23" t="s">
+        <v>8</v>
+      </c>
+      <c r="V23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>8</v>
-      </c>
-      <c r="U23" t="s">
-        <v>8</v>
-      </c>
-      <c r="V23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P24" t="s">
+        <v>8</v>
+      </c>
+      <c r="U24" t="s">
+        <v>8</v>
+      </c>
+      <c r="W24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" t="s">
-        <v>8</v>
-      </c>
-      <c r="P24" t="s">
-        <v>8</v>
-      </c>
-      <c r="U24" t="s">
-        <v>8</v>
-      </c>
-      <c r="W24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="P25" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>8</v>
+      </c>
+      <c r="R25" t="s">
+        <v>8</v>
+      </c>
+      <c r="U25" t="s">
+        <v>8</v>
+      </c>
+      <c r="V25" t="s">
+        <v>8</v>
+      </c>
+      <c r="X25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" t="s">
-        <v>8</v>
-      </c>
-      <c r="P25" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>8</v>
-      </c>
-      <c r="R25" t="s">
-        <v>8</v>
-      </c>
-      <c r="U25" t="s">
-        <v>8</v>
-      </c>
-      <c r="V25" t="s">
-        <v>8</v>
-      </c>
-      <c r="X25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" t="s">
+        <v>8</v>
+      </c>
+      <c r="P26" t="s">
+        <v>8</v>
+      </c>
+      <c r="R26" t="s">
+        <v>8</v>
+      </c>
+      <c r="X26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+      <c r="O27" t="s">
+        <v>8</v>
+      </c>
+      <c r="S27" t="s">
+        <v>8</v>
+      </c>
+      <c r="T27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" t="s">
-        <v>8</v>
-      </c>
-      <c r="P26" t="s">
-        <v>8</v>
-      </c>
-      <c r="R26" t="s">
-        <v>8</v>
-      </c>
-      <c r="X26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" t="s">
-        <v>8</v>
-      </c>
-      <c r="M27" t="s">
-        <v>8</v>
-      </c>
-      <c r="O27" t="s">
-        <v>8</v>
-      </c>
-      <c r="S27" t="s">
-        <v>8</v>
-      </c>
-      <c r="T27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -4230,15 +4230,15 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4426,36 +4426,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
         <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N5" t="s">
         <v>21</v>
@@ -4464,27 +4464,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
         <v>14</v>
@@ -4499,10 +4499,10 @@
         <v>13</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -4664,17 +4664,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -4745,12 +4745,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -4804,91 +4804,91 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" t="s">
+        <v>8</v>
+      </c>
+      <c r="O24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" t="s">
-        <v>8</v>
-      </c>
-      <c r="O24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>8</v>
+      </c>
+      <c r="N25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" t="s">
-        <v>8</v>
-      </c>
-      <c r="N25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" t="s">
-        <v>8</v>
-      </c>
-      <c r="M27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -4915,16 +4915,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC687FA-8034-9347-AA2E-0A9C4F2284C2}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5100,33 +5100,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5140,10 +5140,10 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M6" t="s">
         <v>23</v>
@@ -5152,7 +5152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -5166,7 +5166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -5189,12 +5189,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -5254,17 +5254,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -5329,12 +5329,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -5400,121 +5400,121 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" t="s">
-        <v>8</v>
-      </c>
-      <c r="N24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" t="s">
-        <v>8</v>
-      </c>
-      <c r="J27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" t="s">
-        <v>8</v>
-      </c>
-      <c r="M27" t="s">
-        <v>8</v>
-      </c>
-      <c r="N27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -5537,5 +5537,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>